<commit_message>
Added results for Random Forest
</commit_message>
<xml_diff>
--- a/results/Machine Learning Results.xlsx
+++ b/results/Machine Learning Results.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kazia\Desktop\Python Udemy\GitRepo\CS3IP\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{36F6F7B6-A02C-44DB-A473-266F2DE2B164}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21C4709E-4515-4A10-B1E5-80169DD6E605}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9A48BAD5-1390-4A6E-955D-4139CCF62677}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Dep or Non-Dep Without LOSOCV" sheetId="1" r:id="rId1"/>
+    <sheet name="Dep or Non-Dep With LOSOCV" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,21 +37,54 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>Machine Learning Experiment Results</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="13">
   <si>
     <t>ML model</t>
   </si>
   <si>
     <t>Accuracy</t>
+  </si>
+  <si>
+    <t>Precision</t>
+  </si>
+  <si>
+    <t>Depression/Non-Depression Classification with gender, age and work features</t>
+  </si>
+  <si>
+    <t>Recall</t>
+  </si>
+  <si>
+    <t>F1 Score</t>
+  </si>
+  <si>
+    <t>Balanced Accuracy</t>
+  </si>
+  <si>
+    <t>Random Forest</t>
+  </si>
+  <si>
+    <t>K-Nearest Neighbours</t>
+  </si>
+  <si>
+    <t>Support Vector Machine</t>
+  </si>
+  <si>
+    <t>Depression/Non-Depression Classification without gender, age and work features</t>
+  </si>
+  <si>
+    <t>Machine Learning - Depression/Non-Depression Classification Results (without Leave One Subject Out Cross Validation)</t>
+  </si>
+  <si>
+    <t>Machine Learning - Depression/Non-Depression Classification Results (with Leave One Subject Out Cross Validation)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="172" formatCode="0.000000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -68,7 +102,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -84,6 +118,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -115,12 +155,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -455,34 +500,367 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C105E591-87E0-4C25-B66F-267C25966BD7}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" customWidth="1"/>
+    <col min="6" max="6" width="16.88671875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="4">
+        <v>0.91566265060240903</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0.93548387096774099</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0.85294117647058798</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0.89230769230769202</v>
+      </c>
+      <c r="F5" s="5">
+        <v>0.90606242496998801</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="4">
+        <v>0.73493975903614395</v>
+      </c>
+      <c r="C12" s="4">
+        <v>0.73076923076922995</v>
+      </c>
+      <c r="D12" s="4">
+        <v>0.55882352941176405</v>
+      </c>
+      <c r="E12" s="4">
+        <v>0.63333333333333297</v>
+      </c>
+      <c r="F12" s="5">
+        <v>0.70798319327730996</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:E1"/>
+  <mergeCells count="3">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A3:I3"/>
+    <mergeCell ref="A10:I10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDE22236-43C4-4BB7-A7A8-5429318DC359}">
+  <dimension ref="A1:I14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:I1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="4">
+        <v>0.84169355896628595</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0.36363636363636298</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0.32495474222746901</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0.33904686488418501</v>
+      </c>
+      <c r="F5" s="5">
+        <v>0.84169355896628595</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="4">
+        <v>0.74025449298176504</v>
+      </c>
+      <c r="C12" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="D12" s="4">
+        <v>0.23816214088941301</v>
+      </c>
+      <c r="E12" s="4">
+        <v>0.28096792096792</v>
+      </c>
+      <c r="F12" s="5">
+        <v>0.74025449298176504</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A3:I3"/>
+    <mergeCell ref="A10:I10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added results for K-Nearest Neighbours
</commit_message>
<xml_diff>
--- a/results/Machine Learning Results.xlsx
+++ b/results/Machine Learning Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kazia\Desktop\Python Udemy\GitRepo\CS3IP\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21C4709E-4515-4A10-B1E5-80169DD6E605}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C44640A-3317-473C-AD66-793DCEB47E17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9A48BAD5-1390-4A6E-955D-4139CCF62677}"/>
   </bookViews>
@@ -72,10 +72,10 @@
     <t>Depression/Non-Depression Classification without gender, age and work features</t>
   </si>
   <si>
-    <t>Machine Learning - Depression/Non-Depression Classification Results (without Leave One Subject Out Cross Validation)</t>
-  </si>
-  <si>
-    <t>Machine Learning - Depression/Non-Depression Classification Results (with Leave One Subject Out Cross Validation)</t>
+    <t>Machine Learning - Depression/Non-Depression Classification (without Leave One Subject Out Cross Validation)</t>
+  </si>
+  <si>
+    <t>Machine Learning - Depression/Non-Depression Classification (with Leave One Subject Out Cross Validation)</t>
   </si>
 </sst>
 </file>
@@ -83,7 +83,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="172" formatCode="0.000000"/>
+    <numFmt numFmtId="164" formatCode="0.000000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -158,14 +158,14 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -514,30 +514,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -560,57 +560,67 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="2">
         <v>0.91566265060240903</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="2">
         <v>0.93548387096774099</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="2">
         <v>0.85294117647058798</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="2">
         <v>0.89230769230769202</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="3">
         <v>0.90606242496998801</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
+      <c r="B6" s="2">
+        <v>0.89156626506024095</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.96296296296296202</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.76470588235294101</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.85245901639344202</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0.87214885954381705</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
@@ -633,44 +643,54 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="3">
         <v>0.73493975903614395</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="2">
         <v>0.73076923076922995</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="2">
         <v>0.55882352941176405</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="2">
         <v>0.63333333333333297</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="3">
         <v>0.70798319327730996</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
+      <c r="B13" s="3">
+        <v>0.72289156626506001</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0.73913043478260798</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0.59649122807017496</v>
+      </c>
+      <c r="F13" s="3">
+        <v>0.68877551020408101</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -698,30 +718,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -744,57 +764,67 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="2">
         <v>0.84169355896628595</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="2">
         <v>0.36363636363636298</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="2">
         <v>0.32495474222746901</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="2">
         <v>0.33904686488418501</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="3">
         <v>0.84169355896628595</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
+      <c r="B6" s="2">
+        <v>0.57269064269064196</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.32727272727272699</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.10047619047619</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.146961826052735</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0.57269064269064196</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
@@ -817,44 +847,54 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="2">
         <v>0.74025449298176504</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="2">
         <v>0.4</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="2">
         <v>0.23816214088941301</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="2">
         <v>0.28096792096792</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="3">
         <v>0.74025449298176504</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
+      <c r="B13" s="2">
+        <v>0.51526271708089799</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0.135491932310114</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0.192604768968405</v>
+      </c>
+      <c r="F13" s="3">
+        <v>0.51526271708089799</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Added results for Support Vector Machine
</commit_message>
<xml_diff>
--- a/results/Machine Learning Results.xlsx
+++ b/results/Machine Learning Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kazia\Desktop\Python Udemy\GitRepo\CS3IP\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C44640A-3317-473C-AD66-793DCEB47E17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B51775B-B818-4707-A5CC-061C7007EC17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9A48BAD5-1390-4A6E-955D-4139CCF62677}"/>
   </bookViews>
@@ -82,8 +82,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000000"/>
+    <numFmt numFmtId="167" formatCode="0.00000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -155,7 +156,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -166,6 +167,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -603,11 +605,21 @@
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
+      <c r="B7" s="2">
+        <v>0.85542168674698704</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.86666666666666603</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.76470588235294101</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.8125</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0.84153661464585805</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
@@ -686,11 +698,21 @@
       <c r="A14" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
+      <c r="B14" s="2">
+        <v>0.74698795180722799</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0.76</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0.55882352941176405</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.644067796610169</v>
+      </c>
+      <c r="F14" s="3">
+        <v>0.71818727490996404</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -807,11 +829,21 @@
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
+      <c r="B7" s="2">
+        <v>0.57816481498299599</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.32727272727272699</v>
+      </c>
+      <c r="D7" s="2">
+        <v>7.75914994096812E-2</v>
+      </c>
+      <c r="E7" s="6">
+        <v>0.12232010413828499</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0.57816481498299599</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
@@ -890,11 +922,21 @@
       <c r="A14" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
+      <c r="B14" s="2">
+        <v>0.56467053148871305</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0.122721369539551</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.18257853257853199</v>
+      </c>
+      <c r="F14" s="3">
+        <v>0.56467053148871305</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Added results for Decision Tree
</commit_message>
<xml_diff>
--- a/results/Machine Learning Results.xlsx
+++ b/results/Machine Learning Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kazia\Desktop\Python Udemy\GitRepo\CS3IP\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B51775B-B818-4707-A5CC-061C7007EC17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC512F27-0F0E-4493-A647-4FFEF7C56644}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9A48BAD5-1390-4A6E-955D-4139CCF62677}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="16">
   <si>
     <t>ML model</t>
   </si>
@@ -76,6 +76,15 @@
   </si>
   <si>
     <t>Machine Learning - Depression/Non-Depression Classification (with Leave One Subject Out Cross Validation)</t>
+  </si>
+  <si>
+    <t>Decision Tree</t>
+  </si>
+  <si>
+    <t>Naïve Bayes</t>
+  </si>
+  <si>
+    <t>AdaBoost</t>
   </si>
 </sst>
 </file>
@@ -84,7 +93,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000000"/>
-    <numFmt numFmtId="167" formatCode="0.00000"/>
+    <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -161,13 +170,13 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -502,7 +511,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C105E591-87E0-4C25-B66F-267C25966BD7}">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:I1"/>
@@ -516,30 +525,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -621,104 +630,184 @@
         <v>0.84153661464585805</v>
       </c>
     </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.89156626506024095</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.85714285714285698</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.88235294117647001</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.86956521739130399</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0.89015606242497003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="3"/>
+    </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="3"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B14" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B15" s="3">
         <v>0.73493975903614395</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C15" s="2">
         <v>0.73076923076922995</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D15" s="2">
         <v>0.55882352941176405</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E15" s="2">
         <v>0.63333333333333297</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F15" s="3">
         <v>0.70798319327730996</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B16" s="3">
         <v>0.72289156626506001</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C16" s="3">
         <v>0.73913043478260798</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D16" s="2">
         <v>0.5</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E16" s="2">
         <v>0.59649122807017496</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F16" s="3">
         <v>0.68877551020408101</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B17" s="2">
         <v>0.74698795180722799</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C17" s="2">
         <v>0.76</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D17" s="2">
         <v>0.55882352941176405</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E17" s="2">
         <v>0.644067796610169</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F17" s="3">
         <v>0.71818727490996404</v>
       </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="2">
+        <v>0.686746987951807</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.58823529411764697</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0.60606060606060597</v>
+      </c>
+      <c r="F18" s="3">
+        <v>0.67166866746698595</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A3:I3"/>
-    <mergeCell ref="A10:I10"/>
+    <mergeCell ref="A13:I13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -727,7 +816,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDE22236-43C4-4BB7-A7A8-5429318DC359}">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:I1"/>
@@ -740,30 +829,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -838,111 +927,191 @@
       <c r="D7" s="2">
         <v>7.75914994096812E-2</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="4">
         <v>0.12232010413828499</v>
       </c>
       <c r="F7" s="3">
         <v>0.57816481498299599</v>
       </c>
     </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.79844135662317395</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.381818181818181</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.33851239669421401</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.350375079465988</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0.79844135662317395</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="3"/>
+    </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="3"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B14" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B15" s="2">
         <v>0.74025449298176504</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C15" s="2">
         <v>0.4</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D15" s="2">
         <v>0.23816214088941301</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E15" s="2">
         <v>0.28096792096792</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F15" s="3">
         <v>0.74025449298176504</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B16" s="2">
         <v>0.51526271708089799</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C16" s="2">
         <v>0.4</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D16" s="2">
         <v>0.135491932310114</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E16" s="2">
         <v>0.192604768968405</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F16" s="3">
         <v>0.51526271708089799</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B17" s="2">
         <v>0.56467053148871305</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C17" s="2">
         <v>0.4</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D17" s="2">
         <v>0.122721369539551</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E17" s="2">
         <v>0.18257853257853199</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F17" s="3">
         <v>0.56467053148871305</v>
       </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="2">
+        <v>0.69697211879029997</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.230578512396694</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0.28082200627655102</v>
+      </c>
+      <c r="F18" s="3">
+        <v>0.69697211879029997</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="3"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A3:I3"/>
-    <mergeCell ref="A10:I10"/>
+    <mergeCell ref="A13:I13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added results for Naive Bayes
</commit_message>
<xml_diff>
--- a/results/Machine Learning Results.xlsx
+++ b/results/Machine Learning Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kazia\Desktop\Python Udemy\GitRepo\CS3IP\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC512F27-0F0E-4493-A647-4FFEF7C56644}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B592E70-1DE7-435F-9876-7C53460E988E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9A48BAD5-1390-4A6E-955D-4139CCF62677}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{9A48BAD5-1390-4A6E-955D-4139CCF62677}"/>
   </bookViews>
   <sheets>
     <sheet name="Dep or Non-Dep Without LOSOCV" sheetId="1" r:id="rId1"/>
@@ -654,11 +654,21 @@
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="3"/>
+      <c r="B9" s="2">
+        <v>0.67469879518072196</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.59459459459459396</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.64705882352941102</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0.61971830985915499</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0.67046818727490998</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
@@ -787,11 +797,21 @@
       <c r="A19" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
+      <c r="B19" s="2">
+        <v>0.67469879518072196</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0.59459459459459396</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0.64705882352941102</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0.61971830985915499</v>
+      </c>
+      <c r="F19" s="3">
+        <v>0.67046818727490998</v>
+      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
@@ -958,11 +978,21 @@
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="3"/>
+      <c r="B9" s="2">
+        <v>0.65558880513425899</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0.304779614325068</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0.33299029253574702</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0.65558880513425899</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
@@ -1091,11 +1121,21 @@
       <c r="A19" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="3"/>
+      <c r="B19" s="2">
+        <v>0.65558880513425899</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="D19" s="4">
+        <v>0.304779614325068</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0.33299029253574702</v>
+      </c>
+      <c r="F19" s="3">
+        <v>0.65558880513425899</v>
+      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">

</xml_diff>

<commit_message>
Added results for AdaBoost
</commit_message>
<xml_diff>
--- a/results/Machine Learning Results.xlsx
+++ b/results/Machine Learning Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kazia\Desktop\Python Udemy\GitRepo\CS3IP\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B592E70-1DE7-435F-9876-7C53460E988E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71654461-4C92-4B06-B5EB-C3350D86E306}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{9A48BAD5-1390-4A6E-955D-4139CCF62677}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9A48BAD5-1390-4A6E-955D-4139CCF62677}"/>
   </bookViews>
   <sheets>
     <sheet name="Dep or Non-Dep Without LOSOCV" sheetId="1" r:id="rId1"/>
@@ -674,11 +674,21 @@
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="3"/>
+      <c r="B10" s="2">
+        <v>0.87951807228915602</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.875</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0.82352941176470495</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.84848484848484795</v>
+      </c>
+      <c r="F10" s="3">
+        <v>0.87094837935173997</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
@@ -817,11 +827,21 @@
       <c r="A20" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
+      <c r="B20" s="2">
+        <v>0.69879518072289104</v>
+      </c>
+      <c r="C20" s="2">
+        <v>0.65517241379310298</v>
+      </c>
+      <c r="D20" s="2">
+        <v>0.55882352941176405</v>
+      </c>
+      <c r="E20" s="2">
+        <v>0.60317460317460303</v>
+      </c>
+      <c r="F20" s="3">
+        <v>0.67737094837935097</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -998,11 +1018,21 @@
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="3"/>
+      <c r="B10" s="2">
+        <v>0.83612402748766301</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.381818181818181</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0.33167847304210901</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.34769674769674702</v>
+      </c>
+      <c r="F10" s="3">
+        <v>0.83612402748766301</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
@@ -1141,11 +1171,21 @@
       <c r="A20" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="3"/>
+      <c r="B20" s="2">
+        <v>0.70496024177842298</v>
+      </c>
+      <c r="C20" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="D20" s="2">
+        <v>0.22222353404171499</v>
+      </c>
+      <c r="E20" s="2">
+        <v>0.26536998355180103</v>
+      </c>
+      <c r="F20" s="3">
+        <v>0.70496024177842298</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Redo the results for Random Forest and KNN
</commit_message>
<xml_diff>
--- a/results/Machine Learning Results.xlsx
+++ b/results/Machine Learning Results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kazia\Desktop\Python Udemy\GitRepo\CS3IP\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71654461-4C92-4B06-B5EB-C3350D86E306}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{231A0474-CDE8-43F3-BB12-1BC1F38FF1CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9A48BAD5-1390-4A6E-955D-4139CCF62677}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{9A48BAD5-1390-4A6E-955D-4139CCF62677}"/>
   </bookViews>
   <sheets>
     <sheet name="Dep or Non-Dep Without LOSOCV" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="18">
   <si>
     <t>ML model</t>
   </si>
@@ -85,15 +85,22 @@
   </si>
   <si>
     <t>AdaBoost</t>
+  </si>
+  <si>
+    <t>Depression/Non-Depression Classification with all temporal features</t>
+  </si>
+  <si>
+    <t>Depression/Non-Depression Classification with feature selection</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000000"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
+    <numFmt numFmtId="173" formatCode="0.0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -165,7 +172,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -177,6 +184,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -539,7 +547,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
@@ -575,19 +583,19 @@
         <v>7</v>
       </c>
       <c r="B5" s="2">
-        <v>0.91566265060240903</v>
+        <v>0.69144058081772997</v>
       </c>
       <c r="C5" s="2">
-        <v>0.93548387096774099</v>
+        <v>0.60032102728731895</v>
       </c>
       <c r="D5" s="2">
-        <v>0.85294117647058798</v>
+        <v>0.40107238605898099</v>
       </c>
       <c r="E5" s="2">
-        <v>0.89230769230769202</v>
+        <v>0.48087431693989002</v>
       </c>
       <c r="F5" s="3">
-        <v>0.90606242496998801</v>
+        <v>0.62662702116840396</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -595,19 +603,19 @@
         <v>8</v>
       </c>
       <c r="B6" s="2">
-        <v>0.89156626506024095</v>
+        <v>0.647688192586931</v>
       </c>
       <c r="C6" s="2">
-        <v>0.96296296296296202</v>
+        <v>0.50735809390329301</v>
       </c>
       <c r="D6" s="2">
-        <v>0.76470588235294101</v>
+        <v>0.38820375335120599</v>
       </c>
       <c r="E6" s="2">
-        <v>0.85245901639344202</v>
+        <v>0.43985419198055797</v>
       </c>
       <c r="F6" s="3">
-        <v>0.87214885954381705</v>
+        <v>0.58976824651828597</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -615,84 +623,54 @@
         <v>9</v>
       </c>
       <c r="B7" s="2">
-        <v>0.85542168674698704</v>
+        <v>0.64367596484524203</v>
       </c>
       <c r="C7" s="2">
-        <v>0.86666666666666603</v>
+        <v>0</v>
       </c>
       <c r="D7" s="2">
-        <v>0.76470588235294101</v>
+        <v>0</v>
       </c>
       <c r="E7" s="2">
-        <v>0.8125</v>
-      </c>
-      <c r="F7" s="3">
-        <v>0.84153661464585805</v>
+        <v>0</v>
+      </c>
+      <c r="F7" s="7">
+        <v>0.5</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="2">
-        <v>0.89156626506024095</v>
-      </c>
-      <c r="C8" s="2">
-        <v>0.85714285714285698</v>
-      </c>
-      <c r="D8" s="2">
-        <v>0.88235294117647001</v>
-      </c>
-      <c r="E8" s="2">
-        <v>0.86956521739130399</v>
-      </c>
-      <c r="F8" s="3">
-        <v>0.89015606242497003</v>
-      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="3"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="2">
-        <v>0.67469879518072196</v>
-      </c>
-      <c r="C9" s="2">
-        <v>0.59459459459459396</v>
-      </c>
-      <c r="D9" s="2">
-        <v>0.64705882352941102</v>
-      </c>
-      <c r="E9" s="2">
-        <v>0.61971830985915499</v>
-      </c>
-      <c r="F9" s="3">
-        <v>0.67046818727490998</v>
-      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="3"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="2">
-        <v>0.87951807228915602</v>
-      </c>
-      <c r="C10" s="2">
-        <v>0.875</v>
-      </c>
-      <c r="D10" s="2">
-        <v>0.82352941176470495</v>
-      </c>
-      <c r="E10" s="2">
-        <v>0.84848484848484795</v>
-      </c>
-      <c r="F10" s="3">
-        <v>0.87094837935173997</v>
-      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="3"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -728,19 +706,19 @@
         <v>7</v>
       </c>
       <c r="B15" s="3">
-        <v>0.73493975903614395</v>
+        <v>0.67233473442873504</v>
       </c>
       <c r="C15" s="2">
-        <v>0.73076923076922995</v>
+        <v>0.55742725880551303</v>
       </c>
       <c r="D15" s="2">
-        <v>0.55882352941176405</v>
+        <v>0.39034852546916798</v>
       </c>
       <c r="E15" s="2">
-        <v>0.63333333333333297</v>
+        <v>0.45916114790286899</v>
       </c>
       <c r="F15" s="3">
-        <v>0.70798319327730996</v>
+        <v>0.60939213153838301</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
@@ -748,100 +726,60 @@
         <v>8</v>
       </c>
       <c r="B16" s="3">
-        <v>0.72289156626506001</v>
+        <v>0.647879251050821</v>
       </c>
       <c r="C16" s="3">
-        <v>0.73913043478260798</v>
+        <v>0.50784593437945702</v>
       </c>
       <c r="D16" s="2">
-        <v>0.5</v>
+        <v>0.38176943699731902</v>
       </c>
       <c r="E16" s="2">
-        <v>0.59649122807017496</v>
+        <v>0.43587389041934499</v>
       </c>
       <c r="F16" s="3">
-        <v>0.68877551020408101</v>
+        <v>0.58848044423329804</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="2">
-        <v>0.74698795180722799</v>
-      </c>
-      <c r="C17" s="2">
-        <v>0.76</v>
-      </c>
-      <c r="D17" s="2">
-        <v>0.55882352941176405</v>
-      </c>
-      <c r="E17" s="2">
-        <v>0.644067796610169</v>
-      </c>
-      <c r="F17" s="3">
-        <v>0.71818727490996404</v>
-      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="3"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="2">
-        <v>0.686746987951807</v>
-      </c>
-      <c r="C18" s="2">
-        <v>0.625</v>
-      </c>
-      <c r="D18" s="2">
-        <v>0.58823529411764697</v>
-      </c>
-      <c r="E18" s="2">
-        <v>0.60606060606060597</v>
-      </c>
-      <c r="F18" s="3">
-        <v>0.67166866746698595</v>
-      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="3"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="2">
-        <v>0.67469879518072196</v>
-      </c>
-      <c r="C19" s="2">
-        <v>0.59459459459459396</v>
-      </c>
-      <c r="D19" s="2">
-        <v>0.64705882352941102</v>
-      </c>
-      <c r="E19" s="2">
-        <v>0.61971830985915499</v>
-      </c>
-      <c r="F19" s="3">
-        <v>0.67046818727490998</v>
-      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="3"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="2">
-        <v>0.69879518072289104</v>
-      </c>
-      <c r="C20" s="2">
-        <v>0.65517241379310298</v>
-      </c>
-      <c r="D20" s="2">
-        <v>0.55882352941176405</v>
-      </c>
-      <c r="E20" s="2">
-        <v>0.60317460317460303</v>
-      </c>
-      <c r="F20" s="3">
-        <v>0.67737094837935097</v>
-      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -919,19 +857,19 @@
         <v>7</v>
       </c>
       <c r="B5" s="2">
-        <v>0.84169355896628595</v>
+        <v>0.60813489258062603</v>
       </c>
       <c r="C5" s="2">
-        <v>0.36363636363636298</v>
+        <v>0.41818181818181799</v>
       </c>
       <c r="D5" s="2">
-        <v>0.32495474222746901</v>
+        <v>0.13853297896702699</v>
       </c>
       <c r="E5" s="2">
-        <v>0.33904686488418501</v>
+        <v>0.20185682737924099</v>
       </c>
       <c r="F5" s="3">
-        <v>0.84169355896628595</v>
+        <v>0.60813489258062603</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -939,100 +877,60 @@
         <v>8</v>
       </c>
       <c r="B6" s="2">
-        <v>0.57269064269064196</v>
+        <v>0.54367002752932303</v>
       </c>
       <c r="C6" s="2">
-        <v>0.32727272727272699</v>
+        <v>0.41818181818181799</v>
       </c>
       <c r="D6" s="2">
-        <v>0.10047619047619</v>
+        <v>0.14819598480382101</v>
       </c>
       <c r="E6" s="2">
-        <v>0.146961826052735</v>
-      </c>
-      <c r="F6" s="3">
-        <v>0.57269064269064196</v>
+        <v>0.21754541989269699</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0.54367002752932303</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="2">
-        <v>0.57816481498299599</v>
-      </c>
-      <c r="C7" s="2">
-        <v>0.32727272727272699</v>
-      </c>
-      <c r="D7" s="2">
-        <v>7.75914994096812E-2</v>
-      </c>
-      <c r="E7" s="4">
-        <v>0.12232010413828499</v>
-      </c>
-      <c r="F7" s="3">
-        <v>0.57816481498299599</v>
-      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="3"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="2">
-        <v>0.79844135662317395</v>
-      </c>
-      <c r="C8" s="2">
-        <v>0.381818181818181</v>
-      </c>
-      <c r="D8" s="2">
-        <v>0.33851239669421401</v>
-      </c>
-      <c r="E8" s="2">
-        <v>0.350375079465988</v>
-      </c>
-      <c r="F8" s="3">
-        <v>0.79844135662317395</v>
-      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="3"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="2">
-        <v>0.65558880513425899</v>
-      </c>
-      <c r="C9" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="D9" s="4">
-        <v>0.304779614325068</v>
-      </c>
-      <c r="E9" s="2">
-        <v>0.33299029253574702</v>
-      </c>
-      <c r="F9" s="3">
-        <v>0.65558880513425899</v>
-      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="3"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="2">
-        <v>0.83612402748766301</v>
-      </c>
-      <c r="C10" s="2">
-        <v>0.381818181818181</v>
-      </c>
-      <c r="D10" s="2">
-        <v>0.33167847304210901</v>
-      </c>
-      <c r="E10" s="2">
-        <v>0.34769674769674702</v>
-      </c>
-      <c r="F10" s="3">
-        <v>0.83612402748766301</v>
-      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="3"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
@@ -1072,19 +970,19 @@
         <v>7</v>
       </c>
       <c r="B15" s="2">
-        <v>0.74025449298176504</v>
+        <v>0.595048989455223</v>
       </c>
       <c r="C15" s="2">
-        <v>0.4</v>
+        <v>0.41818181818181799</v>
       </c>
       <c r="D15" s="2">
-        <v>0.23816214088941301</v>
+        <v>0.14251313627492901</v>
       </c>
       <c r="E15" s="2">
-        <v>0.28096792096792</v>
+        <v>0.20779761676101999</v>
       </c>
       <c r="F15" s="3">
-        <v>0.74025449298176504</v>
+        <v>0.595048989455223</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
@@ -1092,100 +990,60 @@
         <v>8</v>
       </c>
       <c r="B16" s="2">
-        <v>0.51526271708089799</v>
+        <v>0.54687729314767897</v>
       </c>
       <c r="C16" s="2">
-        <v>0.4</v>
+        <v>0.41818181818181799</v>
       </c>
       <c r="D16" s="2">
-        <v>0.135491932310114</v>
+        <v>0.149612988247835</v>
       </c>
       <c r="E16" s="2">
-        <v>0.192604768968405</v>
+        <v>0.218975170924364</v>
       </c>
       <c r="F16" s="3">
-        <v>0.51526271708089799</v>
+        <v>0.54687729314767897</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="2">
-        <v>0.56467053148871305</v>
-      </c>
-      <c r="C17" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="D17" s="2">
-        <v>0.122721369539551</v>
-      </c>
-      <c r="E17" s="2">
-        <v>0.18257853257853199</v>
-      </c>
-      <c r="F17" s="3">
-        <v>0.56467053148871305</v>
-      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="3"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="2">
-        <v>0.69697211879029997</v>
-      </c>
-      <c r="C18" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="D18" s="2">
-        <v>0.230578512396694</v>
-      </c>
-      <c r="E18" s="2">
-        <v>0.28082200627655102</v>
-      </c>
-      <c r="F18" s="3">
-        <v>0.69697211879029997</v>
-      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="3"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="2">
-        <v>0.65558880513425899</v>
-      </c>
-      <c r="C19" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="D19" s="4">
-        <v>0.304779614325068</v>
-      </c>
-      <c r="E19" s="2">
-        <v>0.33299029253574702</v>
-      </c>
-      <c r="F19" s="3">
-        <v>0.65558880513425899</v>
-      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="3"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="2">
-        <v>0.70496024177842298</v>
-      </c>
-      <c r="C20" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="D20" s="2">
-        <v>0.22222353404171499</v>
-      </c>
-      <c r="E20" s="2">
-        <v>0.26536998355180103</v>
-      </c>
-      <c r="F20" s="3">
-        <v>0.70496024177842298</v>
-      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Provided the results for the Decision Tree, Naive Bayes and AdaBoost models
</commit_message>
<xml_diff>
--- a/results/Machine Learning Results.xlsx
+++ b/results/Machine Learning Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kazia\Desktop\Python Udemy\GitRepo\CS3IP\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{231A0474-CDE8-43F3-BB12-1BC1F38FF1CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1883FB1-497C-4B43-B3BE-6591C80E6385}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{9A48BAD5-1390-4A6E-955D-4139CCF62677}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9A48BAD5-1390-4A6E-955D-4139CCF62677}"/>
   </bookViews>
   <sheets>
     <sheet name="Dep or Non-Dep Without LOSOCV" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="15">
   <si>
     <t>ML model</t>
   </si>
@@ -48,9 +48,6 @@
     <t>Precision</t>
   </si>
   <si>
-    <t>Depression/Non-Depression Classification with gender, age and work features</t>
-  </si>
-  <si>
     <t>Recall</t>
   </si>
   <si>
@@ -64,12 +61,6 @@
   </si>
   <si>
     <t>K-Nearest Neighbours</t>
-  </si>
-  <si>
-    <t>Support Vector Machine</t>
-  </si>
-  <si>
-    <t>Depression/Non-Depression Classification without gender, age and work features</t>
   </si>
   <si>
     <t>Machine Learning - Depression/Non-Depression Classification (without Leave One Subject Out Cross Validation)</t>
@@ -97,10 +88,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.000000"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
-    <numFmt numFmtId="173" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="171" formatCode="0.0000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -172,19 +164,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -519,7 +513,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C105E591-87E0-4C25-B66F-267C25966BD7}">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:I1"/>
@@ -533,30 +527,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
+      <c r="A1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
+      <c r="A3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -569,18 +563,18 @@
         <v>2</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="2">
         <v>0.69144058081772997</v>
@@ -600,7 +594,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" s="2">
         <v>0.647688192586931</v>
@@ -620,85 +614,115 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B7" s="2">
-        <v>0.64367596484524203</v>
+        <v>0.62762705387848605</v>
       </c>
       <c r="C7" s="2">
-        <v>0</v>
+        <v>0.47514792899408198</v>
       </c>
       <c r="D7" s="2">
-        <v>0</v>
+        <v>0.43056300268096498</v>
       </c>
       <c r="E7" s="2">
-        <v>0</v>
-      </c>
-      <c r="F7" s="7">
-        <v>0.5</v>
+        <v>0.45175808720112498</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0.58364006471240304</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="3"/>
+        <v>11</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.47382499044707599</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.38783749684582303</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.82412868632707703</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.52745367192862003</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0.55201685132619804</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0.68112342376767199</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.58703374777975104</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.35442359249329702</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0.441992644600468</v>
+      </c>
+      <c r="F9" s="8">
+        <v>0.60820022011129704</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="3"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="3"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
+      <c r="A13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F14" s="1" t="s">
+      <c r="A14" s="2" t="s">
         <v>6</v>
+      </c>
+      <c r="B14" s="3">
+        <v>0.67233473442873504</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0.55742725880551303</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0.39034852546916798</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.45916114790286899</v>
+      </c>
+      <c r="F14" s="3">
+        <v>0.60939213153838301</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -706,86 +730,86 @@
         <v>7</v>
       </c>
       <c r="B15" s="3">
-        <v>0.67233473442873504</v>
-      </c>
-      <c r="C15" s="2">
-        <v>0.55742725880551303</v>
+        <v>0.647879251050821</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0.50784593437945702</v>
       </c>
       <c r="D15" s="2">
-        <v>0.39034852546916798</v>
+        <v>0.38176943699731902</v>
       </c>
       <c r="E15" s="2">
-        <v>0.45916114790286899</v>
+        <v>0.43587389041934499</v>
       </c>
       <c r="F15" s="3">
-        <v>0.60939213153838301</v>
+        <v>0.58848044423329804</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" s="3">
-        <v>0.647879251050821</v>
-      </c>
-      <c r="C16" s="3">
-        <v>0.50784593437945702</v>
+        <v>10</v>
+      </c>
+      <c r="B16" s="2">
+        <v>0.62858234619793596</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0.47655786350148299</v>
       </c>
       <c r="D16" s="2">
-        <v>0.38176943699731902</v>
+        <v>0.43056300268096498</v>
       </c>
       <c r="E16" s="2">
-        <v>0.43587389041934499</v>
+        <v>0.45239436619718298</v>
       </c>
       <c r="F16" s="3">
-        <v>0.58848044423329804</v>
+        <v>0.58438212467084705</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="3"/>
+        <v>11</v>
+      </c>
+      <c r="B17" s="2">
+        <v>0.64367596484524203</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0</v>
+      </c>
+      <c r="F17" s="5">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="3"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="3"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="3"/>
+        <v>12</v>
+      </c>
+      <c r="B18" s="2">
+        <v>0.68303400840657202</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0.58848797250859097</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.36729222520107202</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0.45229448662924998</v>
+      </c>
+      <c r="F18" s="3">
+        <v>0.61255676858153896</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A3:I3"/>
-    <mergeCell ref="A13:I13"/>
+    <mergeCell ref="A12:I12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -794,7 +818,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDE22236-43C4-4BB7-A7A8-5429318DC359}">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:I1"/>
@@ -807,30 +831,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
+      <c r="A1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
+      <c r="A3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -843,18 +867,18 @@
         <v>2</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="2">
         <v>0.60813489258062603</v>
@@ -874,7 +898,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" s="2">
         <v>0.54367002752932303</v>
@@ -894,75 +918,115 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="3"/>
+        <v>10</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.56962648750291001</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.41818181818181799</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.169810131400395</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.23960723642450399</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0.56962648750291001</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="3"/>
+        <v>11</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.50654397975994803</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.41818181818181799</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0.33183844080882802</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.36748630065881899</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0.50654397975994803</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0.595119187362253</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.41818181818181799</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.119213404887348</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0.17649801127398901</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0.595119187362253</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="3"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="3"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
+      <c r="A13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F14" s="1" t="s">
+      <c r="A14" s="2" t="s">
         <v>6</v>
+      </c>
+      <c r="B14" s="2">
+        <v>0.595048989455223</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0.41818181818181799</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0.14251313627492901</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.20779761676101999</v>
+      </c>
+      <c r="F14" s="3">
+        <v>0.595048989455223</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -970,86 +1034,86 @@
         <v>7</v>
       </c>
       <c r="B15" s="2">
-        <v>0.595048989455223</v>
+        <v>0.54687729314767897</v>
       </c>
       <c r="C15" s="2">
         <v>0.41818181818181799</v>
       </c>
       <c r="D15" s="2">
-        <v>0.14251313627492901</v>
+        <v>0.149612988247835</v>
       </c>
       <c r="E15" s="2">
-        <v>0.20779761676101999</v>
+        <v>0.218975170924364</v>
       </c>
       <c r="F15" s="3">
-        <v>0.595048989455223</v>
+        <v>0.54687729314767897</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B16" s="2">
-        <v>0.54687729314767897</v>
+        <v>0.56623854203497104</v>
       </c>
       <c r="C16" s="2">
         <v>0.41818181818181799</v>
       </c>
       <c r="D16" s="2">
-        <v>0.149612988247835</v>
+        <v>0.16720594301147601</v>
       </c>
       <c r="E16" s="2">
-        <v>0.218975170924364</v>
+        <v>0.23748447948926199</v>
       </c>
       <c r="F16" s="3">
-        <v>0.54687729314767897</v>
+        <v>0.56623854203497104</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="3"/>
+        <v>11</v>
+      </c>
+      <c r="B17" s="2">
+        <v>0.58181818181818101</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0</v>
+      </c>
+      <c r="D17" s="9">
+        <v>0</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0</v>
+      </c>
+      <c r="F17" s="3">
+        <v>0.58181818181818101</v>
+      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="3"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="3"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="3"/>
+        <v>12</v>
+      </c>
+      <c r="B18" s="2">
+        <v>0.59929946653600996</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0.41818181818181799</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.122726529701398</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0.181955673488543</v>
+      </c>
+      <c r="F18" s="3">
+        <v>0.59929946653600996</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A3:I3"/>
-    <mergeCell ref="A13:I13"/>
+    <mergeCell ref="A12:I12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>